<commit_message>
Adding custom title option to plot roi script.
</commit_message>
<xml_diff>
--- a/Animals_Clearance_Turner_complete_list.xlsx
+++ b/Animals_Clearance_Turner_complete_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rja20/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rja20/Documents/MATLAB/Bruker_radial_recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210C5B3E-A42D-004B-A1C6-E08C4793B9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DAFBF3-D1B6-3E4E-B8C7-6C885F19AE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="660" windowWidth="38560" windowHeight="26700" xr2:uid="{84E1B740-0BA9-6B4F-AA6B-2F5191EC9593}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="178">
   <si>
     <t>Cohort_ID</t>
   </si>
@@ -91,42 +91,12 @@
     <t>Age_Years</t>
   </si>
   <si>
-    <t>Age_Label</t>
-  </si>
-  <si>
-    <t>Specimens ID</t>
-  </si>
-  <si>
-    <t>DWI</t>
-  </si>
-  <si>
-    <t>GRE</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>AgeExVivoMRI</t>
-  </si>
-  <si>
     <t>Diet</t>
   </si>
   <si>
-    <t>Age_Handling</t>
-  </si>
-  <si>
-    <t>Remark</t>
-  </si>
-  <si>
-    <t>Mn2Cl pump</t>
-  </si>
-  <si>
     <t>fMRI</t>
   </si>
   <si>
@@ -304,9 +274,6 @@
     <t>B26011303b</t>
   </si>
   <si>
-    <t>Isotropic T2Rare (scanno 23) is in Bruker folder B26011303, but should be coregistered to thick slice T2Rare (scanno 2) in B26011303b.</t>
-  </si>
-  <si>
     <t>Arunno_or_Crunno</t>
   </si>
   <si>
@@ -593,6 +560,21 @@
   </si>
   <si>
     <t>P26021101</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Block1</t>
+  </si>
+  <si>
+    <t>Block2</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>Isotropic T2Rare (scanno 23) is in Bruker folder B26011303, but should be coregistered to thick slice T2Rare (scanno 2) in B26011303b--did this manually when moving file to 'all_niis', 16 February 2026</t>
   </si>
 </sst>
 </file>
@@ -680,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -694,34 +676,32 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,32 +1039,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS59"/>
+  <dimension ref="A1:AW59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="30" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="0" style="30" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="30"/>
-    <col min="7" max="7" width="15.1640625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" style="30" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="30" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="35" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="30" customWidth="1"/>
-    <col min="13" max="20" width="10.83203125" style="30"/>
-    <col min="21" max="21" width="11.6640625" style="36" customWidth="1"/>
-    <col min="22" max="23" width="11.6640625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="22" style="30" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="30"/>
+    <col min="1" max="1" width="17.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="13" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0" style="13" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="13"/>
+    <col min="7" max="7" width="15.1640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="13" customWidth="1"/>
+    <col min="13" max="24" width="10.83203125" style="13"/>
+    <col min="25" max="25" width="11.6640625" style="17" customWidth="1"/>
+    <col min="26" max="27" width="11.6640625" style="13" customWidth="1"/>
+    <col min="28" max="28" width="22" style="13" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1107,19 +1087,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>8</v>
@@ -1145,80 +1125,56 @@
       <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" s="30" t="s">
+      <c r="U1" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="W1" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="30" t="s">
+      <c r="Y1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC1" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD1" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="30" t="s">
+      <c r="AW1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ1" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1239,47 +1195,47 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-    </row>
-    <row r="3" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+    </row>
+    <row r="3" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K3" s="4">
         <v>46035</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O3" s="4">
         <v>45691</v>
@@ -1299,12 +1255,24 @@
         <f t="shared" ref="T3:T12" si="1">YEARFRAC(O3,Q3)</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U3" s="18"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-    </row>
-    <row r="4" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="36">
+        <v>2</v>
+      </c>
+      <c r="V3" s="36">
+        <v>3</v>
+      </c>
+      <c r="W3" s="36">
+        <v>4</v>
+      </c>
+      <c r="X3" s="36">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+    </row>
+    <row r="4" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1317,59 +1285,57 @@
       <c r="J4" s="3"/>
       <c r="K4" s="4"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="5"/>
       <c r="S4" s="3"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-    </row>
-    <row r="5" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+    </row>
+    <row r="5" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K5" s="4">
         <v>46035</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O5" s="4">
         <v>45691</v>
@@ -1389,87 +1355,115 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U5" s="18"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="X5" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="36">
+        <v>8</v>
+      </c>
+      <c r="V5" s="36">
+        <v>9</v>
+      </c>
+      <c r="W5" s="36">
+        <v>10</v>
+      </c>
+      <c r="X5" s="36">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K6" s="4">
         <v>46035</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="5"/>
       <c r="S6" s="3"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-    </row>
-    <row r="7" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="36">
+        <v>8</v>
+      </c>
+      <c r="V6" s="36">
+        <v>9</v>
+      </c>
+      <c r="W6" s="36">
+        <v>10</v>
+      </c>
+      <c r="X6" s="36">
+        <v>23</v>
+      </c>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+    </row>
+    <row r="7" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K7" s="4">
         <v>46043</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="3"/>
@@ -1477,51 +1471,63 @@
       <c r="R7" s="5"/>
       <c r="S7" s="3"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="36">
+        <v>8</v>
+      </c>
+      <c r="V7" s="36">
+        <v>9</v>
+      </c>
+      <c r="W7" s="36">
+        <v>10</v>
+      </c>
+      <c r="X7" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB7" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="K8" s="4">
         <v>46036</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O8" s="4">
         <v>45691</v>
@@ -1541,43 +1547,55 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U8" s="18"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-    </row>
-    <row r="9" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="36">
+        <v>8</v>
+      </c>
+      <c r="V8" s="36">
+        <v>9</v>
+      </c>
+      <c r="W8" s="36">
+        <v>10</v>
+      </c>
+      <c r="X8" s="36">
+        <v>14</v>
+      </c>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+    </row>
+    <row r="9" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="K9" s="4">
         <v>46051</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="3"/>
@@ -1585,49 +1603,61 @@
       <c r="R9" s="5"/>
       <c r="S9" s="3"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="18">
+      <c r="U9" s="36">
+        <v>8</v>
+      </c>
+      <c r="V9" s="36">
+        <v>9</v>
+      </c>
+      <c r="W9" s="36">
+        <v>10</v>
+      </c>
+      <c r="X9" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="18">
         <v>2</v>
       </c>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-    </row>
-    <row r="10" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+    </row>
+    <row r="10" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K10" s="4">
         <v>46036</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O10" s="4">
         <v>45691</v>
@@ -1647,42 +1677,54 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="14"/>
-      <c r="X10" s="14"/>
-    </row>
-    <row r="11" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="36">
+        <v>8</v>
+      </c>
+      <c r="V10" s="36">
+        <v>9</v>
+      </c>
+      <c r="W10" s="36">
+        <v>10</v>
+      </c>
+      <c r="X10" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="14"/>
+      <c r="AB10" s="14"/>
+    </row>
+    <row r="11" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K11" s="4">
         <v>46044</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="3"/>
@@ -1690,49 +1732,61 @@
       <c r="R11" s="5"/>
       <c r="S11" s="3"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="X11" s="14"/>
-    </row>
-    <row r="12" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="36">
+        <v>8</v>
+      </c>
+      <c r="V11" s="36">
+        <v>9</v>
+      </c>
+      <c r="W11" s="36">
+        <v>10</v>
+      </c>
+      <c r="X11" s="36">
+        <v>23</v>
+      </c>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB11" s="14"/>
+    </row>
+    <row r="12" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K12" s="4">
         <v>46036</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O12" s="4">
         <v>45691</v>
@@ -1752,43 +1806,55 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U12" s="18"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-    </row>
-    <row r="13" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="36">
+        <v>8</v>
+      </c>
+      <c r="V12" s="36">
+        <v>9</v>
+      </c>
+      <c r="W12" s="36">
+        <v>10</v>
+      </c>
+      <c r="X12" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+    </row>
+    <row r="13" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K13" s="4">
         <v>46051</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="3"/>
@@ -1796,49 +1862,61 @@
       <c r="R13" s="5"/>
       <c r="S13" s="3"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="18">
+      <c r="U13" s="36">
+        <v>8</v>
+      </c>
+      <c r="V13" s="36">
+        <v>9</v>
+      </c>
+      <c r="W13" s="36">
+        <v>10</v>
+      </c>
+      <c r="X13" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y13" s="18">
         <v>0</v>
       </c>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-    </row>
-    <row r="14" spans="1:45" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+    </row>
+    <row r="14" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K14" s="4">
         <v>46044</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O14" s="4">
         <v>45691</v>
@@ -1858,14 +1936,26 @@
         <f>YEARFRAC(O14,Q14)</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U14" s="18"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="X14" s="14"/>
-    </row>
-    <row r="15" spans="1:45" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="36">
+        <v>8</v>
+      </c>
+      <c r="V14" s="36">
+        <v>9</v>
+      </c>
+      <c r="W14" s="36">
+        <v>10</v>
+      </c>
+      <c r="X14" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB14" s="14"/>
+    </row>
+    <row r="15" spans="1:49" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1886,47 +1976,51 @@
       <c r="R15" s="8"/>
       <c r="S15" s="6"/>
       <c r="T15" s="8"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-    </row>
-    <row r="16" spans="1:45" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+    </row>
+    <row r="16" spans="1:49" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K16" s="7">
         <v>46037</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O16" s="7">
         <v>45642</v>
@@ -1946,45 +2040,57 @@
         <f>YEARFRAC(O16,Q16)</f>
         <v>1.0805555555555555</v>
       </c>
-      <c r="U16" s="19"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="X16" s="15"/>
-    </row>
-    <row r="17" spans="1:24" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="36">
+        <v>8</v>
+      </c>
+      <c r="V16" s="36">
+        <v>9</v>
+      </c>
+      <c r="W16" s="36">
+        <v>10</v>
+      </c>
+      <c r="X16" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB16" s="15"/>
+    </row>
+    <row r="17" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K17" s="7">
         <v>46052</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O17" s="7"/>
       <c r="P17" s="6"/>
@@ -1992,47 +2098,59 @@
       <c r="R17" s="8"/>
       <c r="S17" s="6"/>
       <c r="T17" s="8"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-    </row>
-    <row r="18" spans="1:24" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="37">
+        <v>8</v>
+      </c>
+      <c r="V17" s="37">
+        <v>9</v>
+      </c>
+      <c r="W17" s="37">
+        <v>10</v>
+      </c>
+      <c r="X17" s="37">
+        <v>7</v>
+      </c>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+    </row>
+    <row r="18" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K18" s="7">
         <v>46052</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O18" s="7">
         <v>45642</v>
@@ -2052,12 +2170,24 @@
         <f>YEARFRAC(O18,Q18)</f>
         <v>1.1222222222222222</v>
       </c>
-      <c r="U18" s="19"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-    </row>
-    <row r="19" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="36">
+        <v>8</v>
+      </c>
+      <c r="V18" s="36">
+        <v>9</v>
+      </c>
+      <c r="W18" s="36">
+        <v>10</v>
+      </c>
+      <c r="X18" s="36">
+        <v>7</v>
+      </c>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+    </row>
+    <row r="19" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2078,47 +2208,51 @@
       <c r="R19" s="11"/>
       <c r="S19" s="9"/>
       <c r="T19" s="11"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="16"/>
-    </row>
-    <row r="20" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="16"/>
+    </row>
+    <row r="20" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K20" s="10">
         <v>46038</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O20" s="10">
         <v>45678</v>
@@ -2138,43 +2272,55 @@
         <f>YEARFRAC(O20,Q20)</f>
         <v>0.98333333333333328</v>
       </c>
-      <c r="U20" s="20"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-    </row>
-    <row r="21" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="38">
+        <v>8</v>
+      </c>
+      <c r="V20" s="38">
+        <v>9</v>
+      </c>
+      <c r="W20" s="38">
+        <v>10</v>
+      </c>
+      <c r="X20" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+    </row>
+    <row r="21" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K21" s="10">
         <v>46057</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O21" s="10"/>
       <c r="P21" s="9">
@@ -2184,49 +2330,61 @@
       <c r="R21" s="11"/>
       <c r="S21" s="9"/>
       <c r="T21" s="11"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="X21" s="16"/>
-    </row>
-    <row r="22" spans="1:24" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="38">
+        <v>8</v>
+      </c>
+      <c r="V21" s="38">
+        <v>9</v>
+      </c>
+      <c r="W21" s="38">
+        <v>10</v>
+      </c>
+      <c r="X21" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB21" s="16"/>
+    </row>
+    <row r="22" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="K22" s="7">
         <v>46052</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="6"/>
@@ -2240,12 +2398,24 @@
         <f>YEARFRAC(O22,Q22)</f>
         <v>0</v>
       </c>
-      <c r="U22" s="19"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-    </row>
-    <row r="23" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="37">
+        <v>8</v>
+      </c>
+      <c r="V22" s="37">
+        <v>9</v>
+      </c>
+      <c r="W22" s="37">
+        <v>10</v>
+      </c>
+      <c r="X22" s="37">
+        <v>7</v>
+      </c>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+    </row>
+    <row r="23" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2266,47 +2436,51 @@
       <c r="R23" s="11"/>
       <c r="S23" s="9"/>
       <c r="T23" s="11"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-    </row>
-    <row r="24" spans="1:24" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+    </row>
+    <row r="24" spans="1:28" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="21" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K24" s="22">
         <v>46037</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O24" s="22">
         <v>45642</v>
@@ -2326,30 +2500,42 @@
         <f>YEARFRAC(O24,Q24)</f>
         <v>1.0805555555555555</v>
       </c>
-      <c r="U24" s="24"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="X24" s="25"/>
-    </row>
-    <row r="25" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="38">
+        <v>8</v>
+      </c>
+      <c r="V24" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="W24" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="X24" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB24" s="25"/>
+    </row>
+    <row r="25" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="26" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="26" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="K25" s="27" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
@@ -2360,47 +2546,51 @@
       <c r="R25" s="11"/>
       <c r="S25" s="9"/>
       <c r="T25" s="11"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-    </row>
-    <row r="26" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+    </row>
+    <row r="26" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="K26" s="10">
         <v>46038</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O26" s="10">
         <v>45719</v>
@@ -2420,43 +2610,55 @@
         <f>YEARFRAC(O26,Q26)</f>
         <v>0.86944444444444446</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-    </row>
-    <row r="27" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="38">
+        <v>8</v>
+      </c>
+      <c r="V26" s="38">
+        <v>9</v>
+      </c>
+      <c r="W26" s="38">
+        <v>10</v>
+      </c>
+      <c r="X26" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="16"/>
+    </row>
+    <row r="27" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="K27" s="10">
         <v>46057</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O27" s="10"/>
       <c r="P27" s="9"/>
@@ -2464,47 +2666,59 @@
       <c r="R27" s="11"/>
       <c r="S27" s="9"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="20"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-    </row>
-    <row r="28" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U27" s="38">
+        <v>8</v>
+      </c>
+      <c r="V27" s="38">
+        <v>14</v>
+      </c>
+      <c r="W27" s="38">
+        <v>10</v>
+      </c>
+      <c r="X27" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+    </row>
+    <row r="28" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="K28" s="10">
         <v>46042</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O28" s="10">
         <v>45293</v>
@@ -2524,12 +2738,24 @@
         <f>YEARFRAC(O28,Q28)</f>
         <v>2.0499999999999998</v>
       </c>
-      <c r="U28" s="20"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-    </row>
-    <row r="29" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U28" s="38">
+        <v>8</v>
+      </c>
+      <c r="V28" s="38">
+        <v>17</v>
+      </c>
+      <c r="W28" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="X28" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="16"/>
+      <c r="AB28" s="16"/>
+    </row>
+    <row r="29" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2550,47 +2776,51 @@
       <c r="R29" s="11"/>
       <c r="S29" s="9"/>
       <c r="T29" s="11"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-    </row>
-    <row r="30" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="16"/>
+      <c r="AB29" s="16"/>
+    </row>
+    <row r="30" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="K30" s="10">
         <v>46038</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O30" s="10">
         <v>45719</v>
@@ -2610,43 +2840,55 @@
         <f>YEARFRAC(O30,Q30)</f>
         <v>0.86944444444444446</v>
       </c>
-      <c r="U30" s="20"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-    </row>
-    <row r="31" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U30" s="38">
+        <v>8</v>
+      </c>
+      <c r="V30" s="38">
+        <v>9</v>
+      </c>
+      <c r="W30" s="38">
+        <v>10</v>
+      </c>
+      <c r="X30" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="16"/>
+      <c r="AB30" s="16"/>
+    </row>
+    <row r="31" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="K31" s="10">
         <v>46062</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O31" s="10"/>
       <c r="P31" s="9">
@@ -2656,49 +2898,61 @@
       <c r="R31" s="11"/>
       <c r="S31" s="9"/>
       <c r="T31" s="11"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="X31" s="16"/>
-    </row>
-    <row r="32" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U31" s="38">
+        <v>8</v>
+      </c>
+      <c r="V31" s="38">
+        <v>9</v>
+      </c>
+      <c r="W31" s="38">
+        <v>24</v>
+      </c>
+      <c r="X31" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB31" s="16"/>
+    </row>
+    <row r="32" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="K32" s="10">
         <v>46042</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O32" s="10">
         <v>45748</v>
@@ -2718,45 +2972,57 @@
         <f>YEARFRAC(O32,Q32)</f>
         <v>0.80277777777777781</v>
       </c>
-      <c r="U32" s="20"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="X32" s="16"/>
-    </row>
-    <row r="33" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U32" s="38">
+        <v>8</v>
+      </c>
+      <c r="V32" s="38">
+        <v>9</v>
+      </c>
+      <c r="W32" s="38">
+        <v>10</v>
+      </c>
+      <c r="X32" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="16"/>
+      <c r="AA32" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB32" s="16"/>
+    </row>
+    <row r="33" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="K33" s="10">
         <v>46063</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O33" s="10"/>
       <c r="P33" s="9">
@@ -2766,51 +3032,63 @@
       <c r="R33" s="11"/>
       <c r="S33" s="9"/>
       <c r="T33" s="11"/>
-      <c r="U33" s="20">
+      <c r="U33" s="38">
         <v>8</v>
       </c>
-      <c r="V33" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="W33" s="16"/>
-      <c r="X33" s="16"/>
-    </row>
-    <row r="34" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V33" s="38">
+        <v>9</v>
+      </c>
+      <c r="W33" s="38">
+        <v>10</v>
+      </c>
+      <c r="X33" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y33" s="20">
+        <v>8</v>
+      </c>
+      <c r="Z33" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
+    </row>
+    <row r="34" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="K34" s="10">
         <v>46042</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O34" s="10">
         <v>45748</v>
@@ -2830,45 +3108,57 @@
         <f>YEARFRAC(O34,Q34)</f>
         <v>0.80277777777777781</v>
       </c>
-      <c r="U34" s="20"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
-      <c r="X34" s="16"/>
-    </row>
-    <row r="35" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U34" s="38">
+        <v>8</v>
+      </c>
+      <c r="V34" s="38">
+        <v>9</v>
+      </c>
+      <c r="W34" s="38">
+        <v>10</v>
+      </c>
+      <c r="X34" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="16"/>
+      <c r="AA34" s="16"/>
+      <c r="AB34" s="16"/>
+    </row>
+    <row r="35" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="K35" s="10">
         <v>46062</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="9"/>
@@ -2876,47 +3166,59 @@
       <c r="R35" s="11"/>
       <c r="S35" s="9"/>
       <c r="T35" s="11"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
-      <c r="X35" s="16"/>
-    </row>
-    <row r="36" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U35" s="38">
+        <v>8</v>
+      </c>
+      <c r="V35" s="38">
+        <v>14</v>
+      </c>
+      <c r="W35" s="38">
+        <v>15</v>
+      </c>
+      <c r="X35" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+    </row>
+    <row r="36" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="K36" s="10">
         <v>46043</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O36" s="10">
         <v>45778</v>
@@ -2936,43 +3238,55 @@
         <f>YEARFRAC(O36,Q36)</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="U36" s="20"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
-      <c r="X36" s="16"/>
-    </row>
-    <row r="37" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U36" s="38">
+        <v>8</v>
+      </c>
+      <c r="V36" s="38">
+        <v>9</v>
+      </c>
+      <c r="W36" s="38">
+        <v>10</v>
+      </c>
+      <c r="X36" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+    </row>
+    <row r="37" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="K37" s="10">
         <v>46057</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O37" s="10"/>
       <c r="P37" s="9"/>
@@ -2980,43 +3294,50 @@
       <c r="R37" s="11"/>
       <c r="S37" s="9"/>
       <c r="T37" s="11"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16"/>
-    </row>
-    <row r="38" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
+      <c r="U37" s="38">
+        <v>8</v>
+      </c>
+      <c r="V37" s="38">
+        <v>9</v>
+      </c>
+      <c r="W37" s="38">
+        <v>10</v>
+      </c>
+      <c r="X37" s="38">
+        <v>7</v>
+      </c>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="16"/>
+      <c r="AB37" s="16"/>
+    </row>
+    <row r="38" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E38" s="28" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>140</v>
+        <v>126</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>129</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="I38" s="28"/>
+        <v>171</v>
+      </c>
       <c r="J38" s="28" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="K38" s="29">
         <v>46063</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M38" s="28" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O38" s="29">
         <v>45748</v>
@@ -3026,47 +3347,53 @@
       </c>
       <c r="Q38" s="29"/>
       <c r="R38" s="16"/>
-      <c r="S38" s="28"/>
       <c r="T38" s="16"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="16"/>
-      <c r="W38" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="X38" s="16"/>
-    </row>
-    <row r="39" spans="1:24" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="U38" s="20">
+        <v>8</v>
+      </c>
+      <c r="V38" s="20">
+        <v>9</v>
+      </c>
+      <c r="W38" s="20">
+        <v>10</v>
+      </c>
+      <c r="X38" s="20">
+        <v>7</v>
+      </c>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB38" s="16"/>
+    </row>
+    <row r="39" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E39" s="28" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>124</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="I39" s="28"/>
+        <v>172</v>
+      </c>
       <c r="J39" s="28" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="K39" s="29">
         <v>46063</v>
       </c>
       <c r="L39" s="28" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M39" s="28" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="O39" s="29">
         <v>45805</v>
@@ -3076,355 +3403,384 @@
       </c>
       <c r="Q39" s="29"/>
       <c r="R39" s="16"/>
-      <c r="S39" s="28"/>
       <c r="T39" s="16"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="16"/>
-      <c r="W39" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="X39" s="16"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="G45" s="30" t="s">
+      <c r="U39" s="20">
+        <v>8</v>
+      </c>
+      <c r="V39" s="20">
+        <v>9</v>
+      </c>
+      <c r="W39" s="20">
+        <v>10</v>
+      </c>
+      <c r="X39" s="20">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB39" s="16"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="K45" s="33">
+        <v>45939</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA45" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K46" s="33">
+        <v>45946</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA46" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="K47" s="33">
+        <v>45960</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA47" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="J45" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="K45" s="35">
-        <v>45939</v>
-      </c>
-      <c r="L45" s="30" t="s">
+      <c r="F48" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="W45" s="30" t="s">
+      <c r="J48" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="K48" s="33">
+        <v>46002</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M48" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N48" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O48" s="33">
+        <v>45761</v>
+      </c>
+      <c r="P48" s="13">
+        <v>28</v>
+      </c>
+      <c r="AA48" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F46" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="J46" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="K46" s="35">
-        <v>45946</v>
-      </c>
-      <c r="L46" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="W46" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="F47" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="G47" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="J47" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="K47" s="35">
-        <v>45960</v>
-      </c>
-      <c r="L47" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="W47" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="J48" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="K48" s="35">
-        <v>46002</v>
-      </c>
-      <c r="L48" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="M48" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="N48" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="O48" s="35">
-        <v>45761</v>
-      </c>
-      <c r="P48" s="30">
-        <v>28</v>
-      </c>
-      <c r="W48" s="30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="F49" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="G49" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="H49" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="J49" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="K49" s="37">
+        <v>41</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="J49" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K49" s="34">
         <v>46002</v>
       </c>
-      <c r="L49" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="M49" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="N49" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="O49" s="37">
+      <c r="L49" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="M49" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O49" s="34">
         <v>45761</v>
       </c>
-      <c r="P49" s="32">
+      <c r="P49" s="31">
         <v>25</v>
       </c>
-      <c r="U49" s="38"/>
-      <c r="W49" s="32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U49" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="V49" s="31">
+        <v>8</v>
+      </c>
+      <c r="W49" s="31">
+        <v>9</v>
+      </c>
+      <c r="X49" s="31">
+        <v>2</v>
+      </c>
+      <c r="Y49" s="19"/>
+      <c r="AA49" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="F50" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="G50" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="H50" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="J50" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="K50" s="37">
+      <c r="J50" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K50" s="34">
         <v>46009</v>
       </c>
-      <c r="L50" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="M50" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="N50" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="P50" s="32">
+      <c r="L50" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="M50" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="U50" s="38"/>
-      <c r="W50" s="32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M54" s="30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M55" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="R55" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="U55" s="30"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="N56" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="P56" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="S56" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="U56" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M57" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="N57" s="30">
+      <c r="N50" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="P50" s="31">
+        <v>27</v>
+      </c>
+      <c r="U50" s="31">
+        <v>13</v>
+      </c>
+      <c r="V50" s="31">
+        <v>22</v>
+      </c>
+      <c r="W50" s="31">
+        <v>9</v>
+      </c>
+      <c r="X50" s="31">
+        <v>2</v>
+      </c>
+      <c r="Y50" s="19"/>
+      <c r="AA50" s="31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M54" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M55" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="R55" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y55" s="13"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="N56" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="P56" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S56" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y56" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M57" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="N57" s="13">
         <v>5</v>
       </c>
-      <c r="O57" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P57" s="30">
+      <c r="O57" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P57" s="13">
         <v>3</v>
       </c>
-      <c r="R57" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="S57" s="30">
+      <c r="R57" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S57" s="13">
         <v>4</v>
       </c>
-      <c r="T57" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="U57" s="30">
+      <c r="T57" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y57" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M58" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="N58" s="30">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M58" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N58" s="13">
         <v>3</v>
       </c>
-      <c r="O58" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="P58" s="30">
+      <c r="O58" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P58" s="13">
         <v>4</v>
       </c>
-      <c r="R58" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="S58" s="30">
+      <c r="R58" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S58" s="13">
         <v>3</v>
       </c>
-      <c r="T58" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="U58" s="30">
+      <c r="T58" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y58" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="M59" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="N59" s="30">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M59" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="N59" s="13">
         <f>SUBTOTAL(9,N57:N58)</f>
         <v>8</v>
       </c>
-      <c r="O59" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="P59" s="30">
+      <c r="O59" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="P59" s="13">
         <f>SUBTOTAL(9,P57:P58)</f>
         <v>7</v>
       </c>
-      <c r="R59" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="S59" s="30">
+      <c r="R59" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="S59" s="13">
         <f>SUBTOTAL(9,S57:S58)</f>
         <v>7</v>
       </c>
-      <c r="T59" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="U59" s="30">
-        <f>SUBTOTAL(9,U57:U58)</f>
+      <c r="T59" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y59" s="13">
+        <f>SUBTOTAL(9,Y57:Y58)</f>
         <v>8</v>
       </c>
     </row>
@@ -3448,87 +3804,87 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Animal list with QA; QA ppt code.
</commit_message>
<xml_diff>
--- a/Animals_Clearance_Turner_complete_list.xlsx
+++ b/Animals_Clearance_Turner_complete_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rja20/Documents/MATLAB/Bruker_radial_recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFB70D8-9968-7B4F-A46B-3FCD4B998EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5495BC5C-E6E3-D344-9E0C-D0CBDC53C699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="8560" windowWidth="38560" windowHeight="26700" xr2:uid="{84E1B740-0BA9-6B4F-AA6B-2F5191EC9593}"/>
+    <workbookView xWindow="4760" yWindow="2100" windowWidth="38560" windowHeight="26700" xr2:uid="{84E1B740-0BA9-6B4F-AA6B-2F5191EC9593}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$B$18</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +34,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="203">
   <si>
     <t>Cohort_ID</t>
   </si>
@@ -590,6 +592,84 @@
   </si>
   <si>
     <t>Slight Possibility It's Usable</t>
+  </si>
+  <si>
+    <t>Needs coregistration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSF never lights up; Extreme motion around 27-30 in block2, may be able to fix by omitting and coregistation (and proper accounting) </t>
+  </si>
+  <si>
+    <t>No dynamics observed; Block2 needs coregistration, volume needs to be thrown out</t>
+  </si>
+  <si>
+    <t>Unusually large ventricles</t>
+  </si>
+  <si>
+    <t>Non-usable</t>
+  </si>
+  <si>
+    <t>Good, but motion in Block1, vols ~22-38 needs to be addressed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Usabl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <t>Still usuble even without block2</t>
+  </si>
+  <si>
+    <t>Last few volumes of Block2 need to be discarded</t>
+  </si>
+  <si>
+    <t>Very good dynamics</t>
+  </si>
+  <si>
+    <t>Significant motion in Block1, omission and coregistration might salvage some data.</t>
+  </si>
+  <si>
+    <t>Possibly usable with good coregistration, etc</t>
+  </si>
+  <si>
+    <t>Interesting dynamics..</t>
+  </si>
+  <si>
+    <t>Block 2 has motion; need coregistration and to throw out some volumes</t>
+  </si>
+  <si>
+    <t>No dynamics??</t>
+  </si>
+  <si>
+    <t>Block2 needs coregistration and omission of some volumes</t>
+  </si>
+  <si>
+    <t>Possibly Usable</t>
+  </si>
+  <si>
+    <t>Ventricles never light up</t>
+  </si>
+  <si>
+    <t>Possibly usable after coregistration</t>
+  </si>
+  <si>
+    <t>Needs coregistration and perhaps omit a few volumes (Block1), dynamics present</t>
   </si>
 </sst>
 </file>
@@ -677,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -713,10 +793,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:AW59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1150,9 @@
     <col min="11" max="11" width="16.33203125" style="33" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" style="13" customWidth="1"/>
     <col min="13" max="24" width="10.83203125" style="13"/>
-    <col min="25" max="25" width="11.6640625" style="17" customWidth="1"/>
-    <col min="26" max="27" width="11.6640625" style="13" customWidth="1"/>
+    <col min="25" max="25" width="26.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" style="13" customWidth="1"/>
     <col min="28" max="28" width="22" style="13" customWidth="1"/>
     <col min="29" max="16384" width="10.83203125" style="13"/>
   </cols>
@@ -1140,16 +1218,16 @@
       <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="W1" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="X1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="Y1" s="17" t="s">
@@ -1210,10 +1288,10 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
     </row>
     <row r="3" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1270,16 +1348,16 @@
         <f t="shared" ref="T3:T12" si="1">YEARFRAC(O3,Q3)</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U3" s="36">
+      <c r="U3" s="18">
         <v>2</v>
       </c>
-      <c r="V3" s="36">
+      <c r="V3" s="18">
         <v>3</v>
       </c>
-      <c r="W3" s="36">
+      <c r="W3" s="18">
         <v>4</v>
       </c>
-      <c r="X3" s="36">
+      <c r="X3" s="18">
         <v>8</v>
       </c>
       <c r="Y3" s="18" t="s">
@@ -1308,10 +1386,10 @@
       <c r="R4" s="5"/>
       <c r="S4" s="3"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
       <c r="Y4" s="18"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="14"/>
@@ -1372,16 +1450,16 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U5" s="36">
+      <c r="U5" s="18">
         <v>8</v>
       </c>
-      <c r="V5" s="36">
+      <c r="V5" s="18">
         <v>9</v>
       </c>
-      <c r="W5" s="36">
+      <c r="W5" s="18">
         <v>10</v>
       </c>
-      <c r="X5" s="36">
+      <c r="X5" s="18">
         <v>2</v>
       </c>
       <c r="Y5" s="18"/>
@@ -1432,20 +1510,24 @@
       <c r="R6" s="5"/>
       <c r="S6" s="3"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="36">
+      <c r="U6" s="18">
         <v>8</v>
       </c>
-      <c r="V6" s="36">
+      <c r="V6" s="18">
         <v>9</v>
       </c>
-      <c r="W6" s="36">
+      <c r="W6" s="18">
         <v>10</v>
       </c>
-      <c r="X6" s="36">
+      <c r="X6" s="18">
         <v>23</v>
       </c>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="14"/>
+      <c r="Y6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>183</v>
+      </c>
       <c r="AA6" s="14"/>
       <c r="AB6" s="14"/>
     </row>
@@ -1488,20 +1570,24 @@
       <c r="R7" s="5"/>
       <c r="S7" s="3"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="36">
+      <c r="U7" s="18">
         <v>8</v>
       </c>
-      <c r="V7" s="36">
+      <c r="V7" s="18">
         <v>9</v>
       </c>
-      <c r="W7" s="36">
+      <c r="W7" s="18">
         <v>10</v>
       </c>
-      <c r="X7" s="36">
+      <c r="X7" s="18">
         <v>7</v>
       </c>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="14"/>
+      <c r="Y7" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>184</v>
+      </c>
       <c r="AA7" s="14" t="s">
         <v>73</v>
       </c>
@@ -1564,20 +1650,24 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U8" s="36">
+      <c r="U8" s="18">
         <v>8</v>
       </c>
-      <c r="V8" s="36">
+      <c r="V8" s="18">
         <v>9</v>
       </c>
-      <c r="W8" s="36">
+      <c r="W8" s="18">
         <v>10</v>
       </c>
-      <c r="X8" s="36">
+      <c r="X8" s="18">
         <v>14</v>
       </c>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="14"/>
+      <c r="Y8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
     </row>
@@ -1620,22 +1710,24 @@
       <c r="R9" s="5"/>
       <c r="S9" s="3"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="36">
+      <c r="U9" s="18">
         <v>8</v>
       </c>
-      <c r="V9" s="36">
+      <c r="V9" s="18">
         <v>9</v>
       </c>
-      <c r="W9" s="36">
+      <c r="W9" s="18">
         <v>10</v>
       </c>
-      <c r="X9" s="36">
+      <c r="X9" s="18">
         <v>7</v>
       </c>
-      <c r="Y9" s="18">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="14"/>
+      <c r="Y9" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>193</v>
+      </c>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
     </row>
@@ -1694,20 +1786,24 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U10" s="36">
+      <c r="U10" s="18">
         <v>8</v>
       </c>
-      <c r="V10" s="36">
+      <c r="V10" s="18">
         <v>9</v>
       </c>
-      <c r="W10" s="36">
+      <c r="W10" s="18">
         <v>10</v>
       </c>
-      <c r="X10" s="36">
+      <c r="X10" s="18">
         <v>7</v>
       </c>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="14"/>
+      <c r="Y10" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z10" s="14" t="s">
+        <v>191</v>
+      </c>
       <c r="AB10" s="14"/>
     </row>
     <row r="11" spans="1:49" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -1749,19 +1845,21 @@
       <c r="R11" s="5"/>
       <c r="S11" s="3"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="36">
+      <c r="U11" s="18">
         <v>8</v>
       </c>
-      <c r="V11" s="36">
+      <c r="V11" s="18">
         <v>9</v>
       </c>
-      <c r="W11" s="36">
+      <c r="W11" s="18">
         <v>10</v>
       </c>
-      <c r="X11" s="36">
+      <c r="X11" s="18">
         <v>23</v>
       </c>
-      <c r="Y11" s="18"/>
+      <c r="Y11" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="Z11" s="14"/>
       <c r="AA11" s="14" t="s">
         <v>78</v>
@@ -1823,20 +1921,24 @@
         <f t="shared" si="1"/>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U12" s="36">
+      <c r="U12" s="18">
         <v>8</v>
       </c>
-      <c r="V12" s="36">
+      <c r="V12" s="18">
         <v>9</v>
       </c>
-      <c r="W12" s="36">
+      <c r="W12" s="18">
         <v>10</v>
       </c>
-      <c r="X12" s="36">
+      <c r="X12" s="18">
         <v>7</v>
       </c>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="14"/>
+      <c r="Y12" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z12" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
     </row>
@@ -1879,22 +1981,24 @@
       <c r="R13" s="5"/>
       <c r="S13" s="3"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="36">
+      <c r="U13" s="18">
         <v>8</v>
       </c>
-      <c r="V13" s="36">
+      <c r="V13" s="18">
         <v>9</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="18">
         <v>10</v>
       </c>
-      <c r="X13" s="36">
+      <c r="X13" s="18">
         <v>7</v>
       </c>
-      <c r="Y13" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="14"/>
+      <c r="Y13" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z13" s="14" t="s">
+        <v>197</v>
+      </c>
       <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
     </row>
@@ -1953,19 +2057,21 @@
         <f>YEARFRAC(O14,Q14)</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="U14" s="36">
+      <c r="U14" s="18">
         <v>8</v>
       </c>
-      <c r="V14" s="36">
+      <c r="V14" s="18">
         <v>9</v>
       </c>
-      <c r="W14" s="36">
+      <c r="W14" s="18">
         <v>10</v>
       </c>
-      <c r="X14" s="36">
+      <c r="X14" s="18">
         <v>7</v>
       </c>
-      <c r="Y14" s="18"/>
+      <c r="Y14" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="Z14" s="14"/>
       <c r="AA14" s="14" t="s">
         <v>82</v>
@@ -1993,10 +2099,10 @@
       <c r="R15" s="8"/>
       <c r="S15" s="6"/>
       <c r="T15" s="8"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
       <c r="Z15" s="15"/>
       <c r="AA15" s="15"/>
@@ -2057,20 +2163,24 @@
         <f>YEARFRAC(O16,Q16)</f>
         <v>1.0805555555555555</v>
       </c>
-      <c r="U16" s="36">
+      <c r="U16" s="18">
         <v>8</v>
       </c>
-      <c r="V16" s="36">
+      <c r="V16" s="18">
         <v>9</v>
       </c>
-      <c r="W16" s="36">
+      <c r="W16" s="18">
         <v>10</v>
       </c>
-      <c r="X16" s="36">
+      <c r="X16" s="18">
         <v>7</v>
       </c>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="15"/>
+      <c r="Y16" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z16" s="15" t="s">
+        <v>196</v>
+      </c>
       <c r="AA16" s="15" t="s">
         <v>93</v>
       </c>
@@ -2115,19 +2225,21 @@
       <c r="R17" s="8"/>
       <c r="S17" s="6"/>
       <c r="T17" s="8"/>
-      <c r="U17" s="37">
+      <c r="U17" s="19">
         <v>8</v>
       </c>
-      <c r="V17" s="37">
+      <c r="V17" s="19">
         <v>9</v>
       </c>
-      <c r="W17" s="37">
+      <c r="W17" s="19">
         <v>10</v>
       </c>
-      <c r="X17" s="37">
+      <c r="X17" s="19">
         <v>7</v>
       </c>
-      <c r="Y17" s="19"/>
+      <c r="Y17" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="Z17" s="15"/>
       <c r="AA17" s="15"/>
       <c r="AB17" s="15"/>
@@ -2187,20 +2299,24 @@
         <f>YEARFRAC(O18,Q18)</f>
         <v>1.1222222222222222</v>
       </c>
-      <c r="U18" s="36">
+      <c r="U18" s="18">
         <v>8</v>
       </c>
-      <c r="V18" s="36">
+      <c r="V18" s="18">
         <v>9</v>
       </c>
-      <c r="W18" s="36">
+      <c r="W18" s="18">
         <v>10</v>
       </c>
-      <c r="X18" s="36">
+      <c r="X18" s="18">
         <v>7</v>
       </c>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="15"/>
+      <c r="Y18" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>200</v>
+      </c>
       <c r="AA18" s="15"/>
       <c r="AB18" s="15"/>
     </row>
@@ -2225,10 +2341,10 @@
       <c r="R19" s="11"/>
       <c r="S19" s="9"/>
       <c r="T19" s="11"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
       <c r="Y19" s="20"/>
       <c r="Z19" s="16"/>
       <c r="AA19" s="16"/>
@@ -2289,19 +2405,19 @@
         <f>YEARFRAC(O20,Q20)</f>
         <v>0.98333333333333328</v>
       </c>
-      <c r="U20" s="38">
+      <c r="U20" s="20">
         <v>8</v>
       </c>
-      <c r="V20" s="38">
+      <c r="V20" s="20">
         <v>9</v>
       </c>
-      <c r="W20" s="38">
+      <c r="W20" s="20">
         <v>10</v>
       </c>
-      <c r="X20" s="38">
+      <c r="X20" s="20">
         <v>7</v>
       </c>
-      <c r="Y20" s="20" t="s">
+      <c r="Y20" s="24" t="s">
         <v>178</v>
       </c>
       <c r="Z20" s="16"/>
@@ -2349,16 +2465,16 @@
       <c r="R21" s="11"/>
       <c r="S21" s="9"/>
       <c r="T21" s="11"/>
-      <c r="U21" s="38">
+      <c r="U21" s="20">
         <v>8</v>
       </c>
-      <c r="V21" s="38">
+      <c r="V21" s="20">
         <v>9</v>
       </c>
-      <c r="W21" s="38">
+      <c r="W21" s="20">
         <v>10</v>
       </c>
-      <c r="X21" s="38">
+      <c r="X21" s="20">
         <v>7</v>
       </c>
       <c r="Y21" s="20" t="s">
@@ -2419,19 +2535,21 @@
         <f>YEARFRAC(O22,Q22)</f>
         <v>0</v>
       </c>
-      <c r="U22" s="37">
+      <c r="U22" s="19">
         <v>8</v>
       </c>
-      <c r="V22" s="37">
+      <c r="V22" s="19">
         <v>9</v>
       </c>
-      <c r="W22" s="37">
+      <c r="W22" s="19">
         <v>10</v>
       </c>
-      <c r="X22" s="37">
+      <c r="X22" s="19">
         <v>7</v>
       </c>
-      <c r="Y22" s="19"/>
+      <c r="Y22" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="Z22" s="15"/>
       <c r="AA22" s="15"/>
       <c r="AB22" s="15"/>
@@ -2457,10 +2575,10 @@
       <c r="R23" s="11"/>
       <c r="S23" s="9"/>
       <c r="T23" s="11"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="38"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
       <c r="Y23" s="20"/>
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
@@ -2521,19 +2639,21 @@
         <f>YEARFRAC(O24,Q24)</f>
         <v>1.0805555555555555</v>
       </c>
-      <c r="U24" s="38">
+      <c r="U24" s="20">
         <v>8</v>
       </c>
-      <c r="V24" s="38" t="s">
+      <c r="V24" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="W24" s="38" t="s">
+      <c r="W24" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="X24" s="38">
+      <c r="X24" s="20">
         <v>7</v>
       </c>
-      <c r="Y24" s="24"/>
+      <c r="Y24" s="20" t="s">
+        <v>187</v>
+      </c>
       <c r="Z24" s="25"/>
       <c r="AA24" s="25" t="s">
         <v>90</v>
@@ -2567,10 +2687,10 @@
       <c r="R25" s="11"/>
       <c r="S25" s="9"/>
       <c r="T25" s="11"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
       <c r="Y25" s="20"/>
       <c r="Z25" s="16"/>
       <c r="AA25" s="16"/>
@@ -2631,19 +2751,19 @@
         <f>YEARFRAC(O26,Q26)</f>
         <v>0.86944444444444446</v>
       </c>
-      <c r="U26" s="38">
+      <c r="U26" s="20">
         <v>8</v>
       </c>
-      <c r="V26" s="38">
+      <c r="V26" s="20">
         <v>9</v>
       </c>
-      <c r="W26" s="38">
+      <c r="W26" s="20">
         <v>10</v>
       </c>
-      <c r="X26" s="38">
+      <c r="X26" s="20">
         <v>7</v>
       </c>
-      <c r="Y26" s="20" t="s">
+      <c r="Y26" s="24" t="s">
         <v>178</v>
       </c>
       <c r="Z26" s="16"/>
@@ -2689,16 +2809,16 @@
       <c r="R27" s="11"/>
       <c r="S27" s="9"/>
       <c r="T27" s="11"/>
-      <c r="U27" s="38">
+      <c r="U27" s="20">
         <v>8</v>
       </c>
-      <c r="V27" s="38">
+      <c r="V27" s="20">
         <v>14</v>
       </c>
-      <c r="W27" s="38">
+      <c r="W27" s="20">
         <v>10</v>
       </c>
-      <c r="X27" s="38">
+      <c r="X27" s="20">
         <v>7</v>
       </c>
       <c r="Y27" s="20" t="s">
@@ -2767,21 +2887,25 @@
         <f>YEARFRAC(O28,Q28)</f>
         <v>2.0499999999999998</v>
       </c>
-      <c r="U28" s="38">
+      <c r="U28" s="20">
         <v>8</v>
       </c>
-      <c r="V28" s="38">
+      <c r="V28" s="20">
         <v>17</v>
       </c>
-      <c r="W28" s="38" t="s">
+      <c r="W28" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="X28" s="38">
+      <c r="X28" s="20">
         <v>7</v>
       </c>
-      <c r="Y28" s="20"/>
+      <c r="Y28" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="Z28" s="16"/>
-      <c r="AA28" s="16"/>
+      <c r="AA28" s="16" t="s">
+        <v>190</v>
+      </c>
       <c r="AB28" s="16"/>
     </row>
     <row r="29" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -2805,10 +2929,10 @@
       <c r="R29" s="11"/>
       <c r="S29" s="9"/>
       <c r="T29" s="11"/>
-      <c r="U29" s="38"/>
-      <c r="V29" s="38"/>
-      <c r="W29" s="38"/>
-      <c r="X29" s="38"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
       <c r="Y29" s="20"/>
       <c r="Z29" s="16"/>
       <c r="AA29" s="16"/>
@@ -2869,20 +2993,24 @@
         <f>YEARFRAC(O30,Q30)</f>
         <v>0.86944444444444446</v>
       </c>
-      <c r="U30" s="38">
+      <c r="U30" s="20">
         <v>8</v>
       </c>
-      <c r="V30" s="38">
+      <c r="V30" s="20">
         <v>9</v>
       </c>
-      <c r="W30" s="38">
+      <c r="W30" s="20">
         <v>10</v>
       </c>
-      <c r="X30" s="38">
+      <c r="X30" s="20">
         <v>7</v>
       </c>
-      <c r="Y30" s="20"/>
-      <c r="Z30" s="16"/>
+      <c r="Y30" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z30" s="16" t="s">
+        <v>185</v>
+      </c>
       <c r="AA30" s="16"/>
       <c r="AB30" s="16"/>
     </row>
@@ -2927,19 +3055,21 @@
       <c r="R31" s="11"/>
       <c r="S31" s="9"/>
       <c r="T31" s="11"/>
-      <c r="U31" s="38">
+      <c r="U31" s="20">
         <v>8</v>
       </c>
-      <c r="V31" s="38">
+      <c r="V31" s="20">
         <v>9</v>
       </c>
-      <c r="W31" s="38">
+      <c r="W31" s="20">
         <v>24</v>
       </c>
-      <c r="X31" s="38">
+      <c r="X31" s="20">
         <v>7</v>
       </c>
-      <c r="Y31" s="20"/>
+      <c r="Y31" s="20" t="s">
+        <v>187</v>
+      </c>
       <c r="Z31" s="16"/>
       <c r="AA31" s="16" t="s">
         <v>107</v>
@@ -3001,19 +3131,21 @@
         <f>YEARFRAC(O32,Q32)</f>
         <v>0.80277777777777781</v>
       </c>
-      <c r="U32" s="38">
+      <c r="U32" s="20">
         <v>8</v>
       </c>
-      <c r="V32" s="38">
+      <c r="V32" s="20">
         <v>9</v>
       </c>
-      <c r="W32" s="38">
+      <c r="W32" s="20">
         <v>10</v>
       </c>
-      <c r="X32" s="38">
+      <c r="X32" s="20">
         <v>7</v>
       </c>
-      <c r="Y32" s="20"/>
+      <c r="Y32" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="Z32" s="16"/>
       <c r="AA32" s="16" t="s">
         <v>113</v>
@@ -3061,25 +3193,27 @@
       <c r="R33" s="11"/>
       <c r="S33" s="9"/>
       <c r="T33" s="11"/>
-      <c r="U33" s="38">
+      <c r="U33" s="20">
         <v>8</v>
       </c>
-      <c r="V33" s="38">
+      <c r="V33" s="20">
         <v>9</v>
       </c>
-      <c r="W33" s="38">
+      <c r="W33" s="20">
         <v>10</v>
       </c>
-      <c r="X33" s="38">
+      <c r="X33" s="20">
         <v>7</v>
       </c>
-      <c r="Y33" s="20">
-        <v>8</v>
+      <c r="Y33" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="Z33" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA33" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="AA33" s="16"/>
       <c r="AB33" s="16"/>
     </row>
     <row r="34" spans="1:28" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3137,19 +3271,21 @@
         <f>YEARFRAC(O34,Q34)</f>
         <v>0.80277777777777781</v>
       </c>
-      <c r="U34" s="38">
+      <c r="U34" s="20">
         <v>8</v>
       </c>
-      <c r="V34" s="38">
+      <c r="V34" s="20">
         <v>9</v>
       </c>
-      <c r="W34" s="38">
+      <c r="W34" s="20">
         <v>10</v>
       </c>
-      <c r="X34" s="38">
+      <c r="X34" s="20">
         <v>7</v>
       </c>
-      <c r="Y34" s="20"/>
+      <c r="Y34" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="Z34" s="16"/>
       <c r="AA34" s="16"/>
       <c r="AB34" s="16"/>
@@ -3195,19 +3331,21 @@
       <c r="R35" s="11"/>
       <c r="S35" s="9"/>
       <c r="T35" s="11"/>
-      <c r="U35" s="38">
+      <c r="U35" s="20">
         <v>8</v>
       </c>
-      <c r="V35" s="38">
+      <c r="V35" s="20">
         <v>14</v>
       </c>
-      <c r="W35" s="38">
+      <c r="W35" s="20">
         <v>15</v>
       </c>
-      <c r="X35" s="38">
+      <c r="X35" s="20">
         <v>7</v>
       </c>
-      <c r="Y35" s="20"/>
+      <c r="Y35" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="Z35" s="16"/>
       <c r="AA35" s="16"/>
       <c r="AB35" s="16"/>
@@ -3267,20 +3405,24 @@
         <f>YEARFRAC(O36,Q36)</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="U36" s="38">
+      <c r="U36" s="20">
         <v>8</v>
       </c>
-      <c r="V36" s="38">
+      <c r="V36" s="20">
         <v>9</v>
       </c>
-      <c r="W36" s="38">
+      <c r="W36" s="20">
         <v>10</v>
       </c>
-      <c r="X36" s="38">
+      <c r="X36" s="20">
         <v>7</v>
       </c>
-      <c r="Y36" s="20"/>
-      <c r="Z36" s="16"/>
+      <c r="Y36" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z36" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="AA36" s="16"/>
       <c r="AB36" s="16"/>
     </row>
@@ -3323,19 +3465,21 @@
       <c r="R37" s="11"/>
       <c r="S37" s="9"/>
       <c r="T37" s="11"/>
-      <c r="U37" s="38">
+      <c r="U37" s="20">
         <v>8</v>
       </c>
-      <c r="V37" s="38">
+      <c r="V37" s="20">
         <v>9</v>
       </c>
-      <c r="W37" s="38">
+      <c r="W37" s="20">
         <v>10</v>
       </c>
-      <c r="X37" s="38">
+      <c r="X37" s="20">
         <v>7</v>
       </c>
-      <c r="Y37" s="20"/>
+      <c r="Y37" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="Z37" s="16"/>
       <c r="AA37" s="16"/>
       <c r="AB37" s="16"/>
@@ -3389,8 +3533,12 @@
       <c r="X38" s="20">
         <v>7</v>
       </c>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="16"/>
+      <c r="Y38" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z38" s="16" t="s">
+        <v>192</v>
+      </c>
       <c r="AA38" s="16" t="s">
         <v>127</v>
       </c>
@@ -3445,8 +3593,12 @@
       <c r="X39" s="20">
         <v>7</v>
       </c>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="16"/>
+      <c r="Y39" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z39" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="AA39" s="16" t="s">
         <v>138</v>
       </c>
@@ -3642,7 +3794,9 @@
       <c r="X49" s="31">
         <v>2</v>
       </c>
-      <c r="Y49" s="19"/>
+      <c r="Y49" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="AA49" s="31" t="s">
         <v>151</v>
       </c>
@@ -3698,7 +3852,9 @@
       <c r="X50" s="31">
         <v>2</v>
       </c>
-      <c r="Y50" s="19"/>
+      <c r="Y50" s="18" t="s">
+        <v>178</v>
+      </c>
       <c r="AA50" s="31" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
Tweaking QA ppt code.
</commit_message>
<xml_diff>
--- a/Animals_Clearance_Turner_complete_list.xlsx
+++ b/Animals_Clearance_Turner_complete_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rja20/Documents/MATLAB/Bruker_radial_recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5495BC5C-E6E3-D344-9E0C-D0CBDC53C699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB4B68-04FA-354D-BB73-A20F009A6AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4760" yWindow="2100" windowWidth="38560" windowHeight="26700" xr2:uid="{84E1B740-0BA9-6B4F-AA6B-2F5191EC9593}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:AW59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>